<commit_message>
inserção e extração de dados não tratados via excel
</commit_message>
<xml_diff>
--- a/excel_integration/teste.xlsx
+++ b/excel_integration/teste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/59326741e45a8639/Área de Trabalho/Serial Experiments/python/sys_gerenciamento/excel_integration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="11_2BB13C84DD01193A6750817247B050B77C6FF365" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54778E48-A330-4777-8C3C-FF973093908B}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_447A879EFAD5AF32BC485AF7992BB6B31962085E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA12ED42-F26D-4F45-916D-FA502C95A34B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gastos" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="9">
   <si>
     <t>ID_Gasto</t>
   </si>
@@ -43,6 +43,12 @@
   <si>
     <t>teste</t>
   </si>
+  <si>
+    <t>teste2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
 </sst>
 </file>
 
@@ -51,7 +57,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,20 +66,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -88,6 +109,117 @@
       <right style="thin">
         <color auto="1"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -100,22 +232,471 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom"/>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom"/>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom"/>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom"/>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom"/>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom"/>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom"/>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom"/>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom"/>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom"/>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom"/>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom"/>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom"/>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -126,6 +707,41 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Gastos" displayName="Gastos" ref="A1:F18" totalsRowShown="0" headerRowDxfId="0" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17">
+  <autoFilter ref="A1:F18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:F6">
+    <sortCondition descending="1" ref="C1:C6"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="ID_Gasto" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID_Sala" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="DataVencimento" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Valor" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Categoria" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Descricao" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Inserir_Gastos" displayName="Inserir_Gastos" ref="A1:E6" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:E6" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E3">
+    <sortCondition descending="1" ref="B1:B3"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID_Sala" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="DataVencimento" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Valor" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Categoria" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Descricao" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -413,98 +1029,350 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="25" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
+        <v>2</v>
+      </c>
+      <c r="C2" s="23">
+        <v>44316</v>
+      </c>
+      <c r="D2" s="19">
+        <v>300</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
-        <v>43939</v>
-      </c>
-      <c r="D2">
-        <v>1250.75</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C3" s="24">
+        <v>43902</v>
+      </c>
+      <c r="D3" s="19">
+        <v>430</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="24">
+        <v>40643</v>
+      </c>
+      <c r="D4" s="19">
+        <v>300</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F4" s="3" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="24">
+        <v>43000</v>
+      </c>
+      <c r="D5" s="19">
+        <v>430</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="24">
+        <v>47617</v>
+      </c>
+      <c r="D6" s="19">
+        <v>300</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="24">
+        <v>46725</v>
+      </c>
+      <c r="D7" s="19">
+        <v>430</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33AF0EB7-A4D6-42E9-BDA9-36A60D57F450}">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21" style="21" customWidth="1"/>
+    <col min="4" max="5" width="21" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="7">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3">
-        <v>43908</v>
-      </c>
-      <c r="C1" s="5">
+      <c r="B1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4">
+        <v>47617</v>
+      </c>
+      <c r="C2" s="19">
         <v>300</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E2" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F10" s="4"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5">
+        <v>46725</v>
+      </c>
+      <c r="C3" s="19">
+        <v>430</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adição de macro EXCEL, xlwings e histórico.
</commit_message>
<xml_diff>
--- a/excel_integration/teste.xlsx
+++ b/excel_integration/teste.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/59326741e45a8639/Área de Trabalho/Serial Experiments/python/sys_gerenciamento/excel_integration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_447A879EFAD5AF32BC485AF7992BB6B31962085E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA12ED42-F26D-4F45-916D-FA502C95A34B}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_539BC86AF18DB3C3892C3846F35D35155712998C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8EF4C55-54B0-4543-9BD3-41B68BD5018A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="150" yWindow="315" windowWidth="15390" windowHeight="13800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gastos" sheetId="1" r:id="rId1"/>
-    <sheet name="Adicionar_Gastos" sheetId="2" r:id="rId2"/>
+    <sheet name="Salas" sheetId="2" r:id="rId2"/>
+    <sheet name="Adicionar_Gastos" sheetId="3" r:id="rId3"/>
+    <sheet name="Home" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>ID_Gasto</t>
   </si>
@@ -41,13 +43,19 @@
     <t>Descricao</t>
   </si>
   <si>
-    <t>teste</t>
+    <t>Pendente</t>
   </si>
   <si>
-    <t>teste2</t>
+    <t>NomeSala</t>
+  </si>
+  <si>
+    <t>ValorTotalGastos</t>
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -57,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +87,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -94,7 +110,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -228,11 +244,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -300,54 +359,51 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="29">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom"/>
@@ -532,6 +588,109 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom"/>
       <border>
@@ -580,6 +739,30 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom"/>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="bottom"/>
       <border>
@@ -694,6 +877,38 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom"/>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -709,36 +924,53 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Gastos" displayName="Gastos" ref="A1:F18" totalsRowShown="0" headerRowDxfId="0" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17">
-  <autoFilter ref="A1:F18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Gastos" displayName="Gastos" ref="A1:G18" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25">
+  <autoFilter ref="A1:G18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:F6">
     <sortCondition descending="1" ref="C1:C6"/>
   </sortState>
-  <tableColumns count="6">
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="ID_Gasto" dataDxfId="16"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID_Sala" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="DataVencimento" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Valor" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Categoria" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Descricao" dataDxfId="11"/>
+  <tableColumns count="7">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="ID_Gasto" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID_Sala" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="DataVencimento" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Valor" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Categoria" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Descricao" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Pendente" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Inserir_Gastos" displayName="Inserir_Gastos" ref="A1:E6" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="A1:E6" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Salas" displayName="Salas" ref="A1:C6" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="A1:C6" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID_Sala" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="NomeSala" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="ValorTotalGastos" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Inserir_Gastos" displayName="Inserir_Gastos" ref="A1:E6" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:E6" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E3">
     <sortCondition descending="1" ref="B1:B3"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID_Sala" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="DataVencimento" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Valor" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Categoria" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Descricao" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="ID_Sala" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="DataVencimento" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Valor" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Categoria" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Descricao" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1029,10 +1261,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,235 +1274,184 @@
     <col min="3" max="3" width="20.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" style="22" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="14" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:7" s="25" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="28" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
-        <v>2</v>
-      </c>
-      <c r="C2" s="23">
-        <v>44316</v>
-      </c>
-      <c r="D2" s="19">
-        <v>300</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="G1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="24">
-        <v>43902</v>
-      </c>
-      <c r="D3" s="19">
-        <v>430</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="24">
-        <v>40643</v>
-      </c>
-      <c r="D4" s="19">
-        <v>300</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="24">
-        <v>43000</v>
-      </c>
-      <c r="D5" s="19">
-        <v>430</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="24">
-        <v>47617</v>
-      </c>
-      <c r="D6" s="19">
-        <v>300</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="24">
-        <v>46725</v>
-      </c>
-      <c r="D7" s="19">
-        <v>430</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="27"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="26"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="26"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="26"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="26"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="26"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="9"/>
       <c r="D8" s="20"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="26"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="5"/>
       <c r="D9" s="19"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="26"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="5"/>
       <c r="D10" s="19"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="26"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="5"/>
       <c r="D11" s="19"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="5"/>
       <c r="D12" s="19"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="26"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="5"/>
       <c r="D13" s="19"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="26"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="5"/>
       <c r="D14" s="19"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="26"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="5"/>
       <c r="D15" s="19"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="26"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="5"/>
       <c r="D16" s="19"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="26"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="5"/>
       <c r="D17" s="19"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="26"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="9"/>
       <c r="D18" s="20"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1282,10 +1463,69 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="35"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="33"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="35"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="33"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="35"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="33"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="35"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="36"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E6" sqref="B1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,37 +1555,21 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
-      <c r="B2" s="4">
-        <v>47617</v>
-      </c>
-      <c r="C2" s="19">
-        <v>300</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>6</v>
-      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
-      <c r="B3" s="5">
-        <v>46725</v>
-      </c>
-      <c r="C3" s="19">
-        <v>430</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>7</v>
-      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="15"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
@@ -1375,4 +1599,16 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>